<commit_message>
Completed Appeal Form Date verification
</commit_message>
<xml_diff>
--- a/Data Files/Eligibility_Data.xlsx
+++ b/Data Files/Eligibility_Data.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CF240E-80B0-426B-9589-6288CE85E8E9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FA8A78-A28E-4A21-A03A-6D8DBEF7B1E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Day</t>
   </si>
@@ -46,7 +54,22 @@
     <t>Date Type</t>
   </si>
   <si>
-    <t>2020</t>
+    <t>8 Weeks</t>
+  </si>
+  <si>
+    <t>12 Weeks</t>
+  </si>
+  <si>
+    <t>5 Weeks</t>
+  </si>
+  <si>
+    <t>6 Months Plus 8 Weeks</t>
+  </si>
+  <si>
+    <t>6 Months Plus 5 Weeks</t>
+  </si>
+  <si>
+    <t>6 Months</t>
   </si>
 </sst>
 </file>
@@ -82,9 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,18 +390,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -389,22 +420,67 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
+      <c r="B2" s="2">
+        <f ca="1">DAY(TODAY())</f>
+        <v>24</v>
+      </c>
+      <c r="C2" s="3" t="str">
+        <f ca="1">TEXT(TODAY(),"mm")</f>
+        <v>03</v>
+      </c>
+      <c r="D2" s="2">
+        <f ca="1">YEAR(TODAY())</f>
+        <v>2020</v>
+      </c>
+      <c r="E2" s="2">
+        <f ca="1">DATEDIF(TODAY(),EDATE(TODAY(),6),"D")</f>
+        <v>184</v>
+      </c>
+      <c r="F2">
+        <f>SUM(8*7)</f>
+        <v>56</v>
+      </c>
+      <c r="G2">
+        <f>SUM(12*7)</f>
+        <v>84</v>
+      </c>
+      <c r="H2">
+        <f>SUM(5*7)</f>
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <f ca="1">SUM(E2+F2)</f>
+        <v>240</v>
+      </c>
+      <c r="J2">
+        <f ca="1">SUM(E2+(5*7))</f>
+        <v>219</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>